<commit_message>
Update seen i2c devices
</commit_message>
<xml_diff>
--- a/VenusAddresses.xlsx
+++ b/VenusAddresses.xlsx
@@ -86,9 +86,6 @@
     <t>7BIT</t>
   </si>
   <si>
-    <t>8BIT</t>
-  </si>
-  <si>
     <t>Device</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>GLOBAL</t>
+  </si>
+  <si>
+    <t>8BIT (7BIT&lt;&lt;1)</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,15 +541,15 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="4" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -599,11 +599,11 @@
         <f t="shared" ref="F3:F18" si="1">DEC2BIN(E3,8)</f>
         <v>00110110</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>23</v>
+      <c r="G3" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -629,11 +629,11 @@
         <f t="shared" si="1"/>
         <v>00111110</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>23</v>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -659,11 +659,11 @@
         <f t="shared" si="1"/>
         <v>01000100</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>22</v>
+      <c r="G5" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -689,11 +689,11 @@
         <f t="shared" si="1"/>
         <v>01001000</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>22</v>
+      <c r="G6" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -719,11 +719,11 @@
         <f t="shared" si="1"/>
         <v>01001010</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>22</v>
+      <c r="G7" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -750,10 +750,10 @@
         <v>01011000</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -803,11 +803,11 @@
         <f t="shared" si="1"/>
         <v>01011110</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>35</v>
+      <c r="G10" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -881,11 +881,11 @@
         <f t="shared" si="1"/>
         <v>10101100</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>23</v>
+      <c r="G13" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -912,10 +912,10 @@
         <v>10101110</v>
       </c>
       <c r="G14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -942,7 +942,7 @@
         <v>10111110</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>18</v>
@@ -971,11 +971,11 @@
         <f t="shared" si="1"/>
         <v>11100100</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>36</v>
+      <c r="G16" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1001,11 +1001,11 @@
         <f t="shared" si="1"/>
         <v>11100110</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1031,11 +1031,11 @@
         <f t="shared" si="1"/>
         <v>11101010</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>23</v>
+      <c r="G18" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>